<commit_message>
Enhance daily stats export with summary statistics and update .gitignore
</commit_message>
<xml_diff>
--- a/activity_summary.xlsx
+++ b/activity_summary.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Daily Totals" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Weekly Totals" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Daily Stats Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,11 +460,15 @@
       <c r="B2" t="n">
         <v>6675</v>
       </c>
-      <c r="C2" t="n">
-        <v>4.89</v>
-      </c>
-      <c r="D2" t="n">
-        <v>309.99</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      4,89</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    309,99</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -475,11 +480,15 @@
       <c r="B3" t="n">
         <v>8812</v>
       </c>
-      <c r="C3" t="n">
-        <v>6.19</v>
-      </c>
-      <c r="D3" t="n">
-        <v>359.34</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      6,19</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    359,34</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -491,11 +500,15 @@
       <c r="B4" t="n">
         <v>25271</v>
       </c>
-      <c r="C4" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1080.11</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     17,50</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1.080,11</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -507,11 +520,15 @@
       <c r="B5" t="n">
         <v>7477</v>
       </c>
-      <c r="C5" t="n">
-        <v>5.18</v>
-      </c>
-      <c r="D5" t="n">
-        <v>307.19</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      5,18</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    307,19</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -523,11 +540,15 @@
       <c r="B6" t="n">
         <v>8092</v>
       </c>
-      <c r="C6" t="n">
-        <v>5.63</v>
-      </c>
-      <c r="D6" t="n">
-        <v>403.13</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      5,63</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    403,13</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -539,11 +560,15 @@
       <c r="B7" t="n">
         <v>19236</v>
       </c>
-      <c r="C7" t="n">
-        <v>13.76</v>
-      </c>
-      <c r="D7" t="n">
-        <v>820.4</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     13,76</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    820,40</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -555,11 +580,15 @@
       <c r="B8" t="n">
         <v>74</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.09</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      0,05</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      1,09</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -571,11 +600,15 @@
       <c r="B9" t="n">
         <v>12877</v>
       </c>
-      <c r="C9" t="n">
-        <v>8.869999999999999</v>
-      </c>
-      <c r="D9" t="n">
-        <v>543.24</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      8,87</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    543,24</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -587,11 +620,15 @@
       <c r="B10" t="n">
         <v>13895</v>
       </c>
-      <c r="C10" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="D10" t="n">
-        <v>564.26</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      9,60</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    564,26</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -603,11 +640,15 @@
       <c r="B11" t="n">
         <v>14566</v>
       </c>
-      <c r="C11" t="n">
-        <v>10.7</v>
-      </c>
-      <c r="D11" t="n">
-        <v>655.79</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,70</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    655,79</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -619,11 +660,15 @@
       <c r="B12" t="n">
         <v>13146</v>
       </c>
-      <c r="C12" t="n">
-        <v>9.390000000000001</v>
-      </c>
-      <c r="D12" t="n">
-        <v>562.6799999999999</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      9,39</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    562,68</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -635,11 +680,15 @@
       <c r="B13" t="n">
         <v>17458</v>
       </c>
-      <c r="C13" t="n">
-        <v>10.19</v>
-      </c>
-      <c r="D13" t="n">
-        <v>562.13</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,19</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    562,13</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -651,11 +700,15 @@
       <c r="B14" t="n">
         <v>22457</v>
       </c>
-      <c r="C14" t="n">
-        <v>15.37</v>
-      </c>
-      <c r="D14" t="n">
-        <v>920.01</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     15,37</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    920,01</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -667,11 +720,15 @@
       <c r="B15" t="n">
         <v>16329</v>
       </c>
-      <c r="C15" t="n">
-        <v>12.24</v>
-      </c>
-      <c r="D15" t="n">
-        <v>784.79</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,24</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    784,79</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -683,11 +740,15 @@
       <c r="B16" t="n">
         <v>15617</v>
       </c>
-      <c r="C16" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="D16" t="n">
-        <v>582.4299999999999</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,27</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    582,43</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -699,11 +760,15 @@
       <c r="B17" t="n">
         <v>17568</v>
       </c>
-      <c r="C17" t="n">
-        <v>11.07</v>
-      </c>
-      <c r="D17" t="n">
-        <v>616.5599999999999</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,07</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    616,56</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -715,11 +780,15 @@
       <c r="B18" t="n">
         <v>18548</v>
       </c>
-      <c r="C18" t="n">
-        <v>12.19</v>
-      </c>
-      <c r="D18" t="n">
-        <v>704.03</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,19</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    704,03</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -731,11 +800,15 @@
       <c r="B19" t="n">
         <v>15700</v>
       </c>
-      <c r="C19" t="n">
-        <v>10.07</v>
-      </c>
-      <c r="D19" t="n">
-        <v>568.03</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,07</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    568,03</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -747,11 +820,15 @@
       <c r="B20" t="n">
         <v>32087</v>
       </c>
-      <c r="C20" t="n">
-        <v>20.91</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1262.85</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     20,91</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1.262,85</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -763,11 +840,15 @@
       <c r="B21" t="n">
         <v>23643</v>
       </c>
-      <c r="C21" t="n">
-        <v>15.64</v>
-      </c>
-      <c r="D21" t="n">
-        <v>871.29</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     15,64</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    871,29</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -779,11 +860,15 @@
       <c r="B22" t="n">
         <v>16850</v>
       </c>
-      <c r="C22" t="n">
-        <v>11.22</v>
-      </c>
-      <c r="D22" t="n">
-        <v>684.8200000000001</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,22</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    684,82</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -795,11 +880,15 @@
       <c r="B23" t="n">
         <v>16441</v>
       </c>
-      <c r="C23" t="n">
-        <v>11.13</v>
-      </c>
-      <c r="D23" t="n">
-        <v>676.47</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,13</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    676,47</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -811,11 +900,15 @@
       <c r="B24" t="n">
         <v>19231</v>
       </c>
-      <c r="C24" t="n">
-        <v>12.91</v>
-      </c>
-      <c r="D24" t="n">
-        <v>746.2</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,91</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    746,20</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -827,11 +920,15 @@
       <c r="B25" t="n">
         <v>18477</v>
       </c>
-      <c r="C25" t="n">
-        <v>11.67</v>
-      </c>
-      <c r="D25" t="n">
-        <v>649.54</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,67</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    649,54</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -843,11 +940,15 @@
       <c r="B26" t="n">
         <v>23487</v>
       </c>
-      <c r="C26" t="n">
-        <v>13.36</v>
-      </c>
-      <c r="D26" t="n">
-        <v>750.35</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     13,36</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    750,35</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -859,11 +960,15 @@
       <c r="B27" t="n">
         <v>24365</v>
       </c>
-      <c r="C27" t="n">
-        <v>14.73</v>
-      </c>
-      <c r="D27" t="n">
-        <v>854.28</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     14,73</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    854,28</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -875,11 +980,15 @@
       <c r="B28" t="n">
         <v>18278</v>
       </c>
-      <c r="C28" t="n">
-        <v>12.53</v>
-      </c>
-      <c r="D28" t="n">
-        <v>724.6799999999999</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,53</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    724,68</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -891,11 +1000,15 @@
       <c r="B29" t="n">
         <v>17731</v>
       </c>
-      <c r="C29" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1007.25</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     14,79</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1.007,25</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -907,11 +1020,15 @@
       <c r="B30" t="n">
         <v>16503</v>
       </c>
-      <c r="C30" t="n">
-        <v>11.05</v>
-      </c>
-      <c r="D30" t="n">
-        <v>639.26</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,05</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    639,26</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -923,11 +1040,15 @@
       <c r="B31" t="n">
         <v>17339</v>
       </c>
-      <c r="C31" t="n">
-        <v>11.08</v>
-      </c>
-      <c r="D31" t="n">
-        <v>656.47</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,08</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    656,47</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -939,11 +1060,15 @@
       <c r="B32" t="n">
         <v>16870</v>
       </c>
-      <c r="C32" t="n">
-        <v>11.46</v>
-      </c>
-      <c r="D32" t="n">
-        <v>693.11</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,46</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    693,11</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -955,11 +1080,15 @@
       <c r="B33" t="n">
         <v>18283</v>
       </c>
-      <c r="C33" t="n">
-        <v>12.2</v>
-      </c>
-      <c r="D33" t="n">
-        <v>714.88</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,20</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    714,88</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -971,11 +1100,15 @@
       <c r="B34" t="n">
         <v>16096</v>
       </c>
-      <c r="C34" t="n">
-        <v>10.72</v>
-      </c>
-      <c r="D34" t="n">
-        <v>636.5599999999999</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,72</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    636,56</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -987,11 +1120,15 @@
       <c r="B35" t="n">
         <v>16322</v>
       </c>
-      <c r="C35" t="n">
-        <v>11.29</v>
-      </c>
-      <c r="D35" t="n">
-        <v>683.8099999999999</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,29</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    683,81</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1003,11 +1140,15 @@
       <c r="B36" t="n">
         <v>17668</v>
       </c>
-      <c r="C36" t="n">
-        <v>13.06</v>
-      </c>
-      <c r="D36" t="n">
-        <v>852.59</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     13,06</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    852,59</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1019,11 +1160,15 @@
       <c r="B37" t="n">
         <v>15609</v>
       </c>
-      <c r="C37" t="n">
-        <v>11.56</v>
-      </c>
-      <c r="D37" t="n">
-        <v>711.92</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,56</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    711,92</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1035,11 +1180,15 @@
       <c r="B38" t="n">
         <v>15371</v>
       </c>
-      <c r="C38" t="n">
-        <v>11.47</v>
-      </c>
-      <c r="D38" t="n">
-        <v>723.13</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,47</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    723,13</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1051,11 +1200,15 @@
       <c r="B39" t="n">
         <v>18069</v>
       </c>
-      <c r="C39" t="n">
-        <v>12.2</v>
-      </c>
-      <c r="D39" t="n">
-        <v>731.36</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,20</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    731,36</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1067,11 +1220,15 @@
       <c r="B40" t="n">
         <v>17349</v>
       </c>
-      <c r="C40" t="n">
-        <v>12.94</v>
-      </c>
-      <c r="D40" t="n">
-        <v>801.01</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,94</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    801,01</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1083,11 +1240,15 @@
       <c r="B41" t="n">
         <v>17609</v>
       </c>
-      <c r="C41" t="n">
-        <v>12.38</v>
-      </c>
-      <c r="D41" t="n">
-        <v>733</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,38</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    733,00</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1099,11 +1260,15 @@
       <c r="B42" t="n">
         <v>14801</v>
       </c>
-      <c r="C42" t="n">
-        <v>10.22</v>
-      </c>
-      <c r="D42" t="n">
-        <v>842.27</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,22</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    842,27</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1115,11 +1280,15 @@
       <c r="B43" t="n">
         <v>18966</v>
       </c>
-      <c r="C43" t="n">
-        <v>13.17</v>
-      </c>
-      <c r="D43" t="n">
-        <v>755.2</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     13,17</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    755,20</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1131,11 +1300,15 @@
       <c r="B44" t="n">
         <v>17973</v>
       </c>
-      <c r="C44" t="n">
-        <v>11.58</v>
-      </c>
-      <c r="D44" t="n">
-        <v>698.96</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,58</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    698,96</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1147,11 +1320,15 @@
       <c r="B45" t="n">
         <v>19664</v>
       </c>
-      <c r="C45" t="n">
-        <v>12.11</v>
-      </c>
-      <c r="D45" t="n">
-        <v>707.38</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,11</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    707,38</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1163,11 +1340,15 @@
       <c r="B46" t="n">
         <v>16354</v>
       </c>
-      <c r="C46" t="n">
-        <v>11.46</v>
-      </c>
-      <c r="D46" t="n">
-        <v>695.1</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,46</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    695,10</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1179,11 +1360,15 @@
       <c r="B47" t="n">
         <v>11800</v>
       </c>
-      <c r="C47" t="n">
-        <v>8.08</v>
-      </c>
-      <c r="D47" t="n">
-        <v>460.1</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      8,08</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    460,10</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1195,11 +1380,15 @@
       <c r="B48" t="n">
         <v>16493</v>
       </c>
-      <c r="C48" t="n">
-        <v>11.76</v>
-      </c>
-      <c r="D48" t="n">
-        <v>722.5700000000001</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,76</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    722,57</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1211,11 +1400,15 @@
       <c r="B49" t="n">
         <v>19353</v>
       </c>
-      <c r="C49" t="n">
-        <v>11.73</v>
-      </c>
-      <c r="D49" t="n">
-        <v>654.8099999999999</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,73</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    654,81</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1227,11 +1420,15 @@
       <c r="B50" t="n">
         <v>19690</v>
       </c>
-      <c r="C50" t="n">
-        <v>12.24</v>
-      </c>
-      <c r="D50" t="n">
-        <v>710.64</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,24</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    710,64</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1243,11 +1440,15 @@
       <c r="B51" t="n">
         <v>9837</v>
       </c>
-      <c r="C51" t="n">
-        <v>6.64</v>
-      </c>
-      <c r="D51" t="n">
-        <v>385.11</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      6,64</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    385,11</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1259,11 +1460,15 @@
       <c r="B52" t="n">
         <v>17625</v>
       </c>
-      <c r="C52" t="n">
-        <v>11.75</v>
-      </c>
-      <c r="D52" t="n">
-        <v>675.84</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,75</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    675,84</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1275,11 +1480,15 @@
       <c r="B53" t="n">
         <v>18404</v>
       </c>
-      <c r="C53" t="n">
-        <v>12.02</v>
-      </c>
-      <c r="D53" t="n">
-        <v>677.5</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     12,02</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    677,50</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1291,11 +1500,15 @@
       <c r="B54" t="n">
         <v>13342</v>
       </c>
-      <c r="C54" t="n">
-        <v>9.06</v>
-      </c>
-      <c r="D54" t="n">
-        <v>541.38</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      9,06</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    541,38</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1307,11 +1520,15 @@
       <c r="B55" t="n">
         <v>8</v>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.05</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      0,00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      0,05</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1370,11 +1587,15 @@
       <c r="B2" t="n">
         <v>75637</v>
       </c>
-      <c r="C2" t="n">
-        <v>53.18</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3281.26</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     53,18</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  3.281,26</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1386,11 +1607,15 @@
       <c r="B3" t="n">
         <v>110728</v>
       </c>
-      <c r="C3" t="n">
-        <v>76.37</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4592.89</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     76,37</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4.592,89</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1402,11 +1627,15 @@
       <c r="B4" t="n">
         <v>140013</v>
       </c>
-      <c r="C4" t="n">
-        <v>91.37</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5290.01</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     91,37</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  5.290,01</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -1418,11 +1647,15 @@
       <c r="B5" t="n">
         <v>138010</v>
       </c>
-      <c r="C5" t="n">
-        <v>91.09999999999999</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5408.76</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     91,10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  5.408,76</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1434,11 +1667,15 @@
       <c r="B6" t="n">
         <v>119081</v>
       </c>
-      <c r="C6" t="n">
-        <v>80.87</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4876.68</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     80,87</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4.876,68</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1450,11 +1687,15 @@
       <c r="B7" t="n">
         <v>117774</v>
       </c>
-      <c r="C7" t="n">
-        <v>83.95</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5297.89</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     83,95</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  5.297,89</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1466,11 +1707,15 @@
       <c r="B8" t="n">
         <v>121327</v>
       </c>
-      <c r="C8" t="n">
-        <v>78.95999999999999</v>
-      </c>
-      <c r="D8" t="n">
-        <v>4649.57</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     78,96</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  4.649,57</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -1482,11 +1727,149 @@
       <c r="B9" t="n">
         <v>59216</v>
       </c>
-      <c r="C9" t="n">
-        <v>39.46</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2279.87</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     39,46</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  2.279,87</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Steps</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 32.087,00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      8,00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17.104,50</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16.329,37</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Distance (km)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     20,91</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      0,00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,51</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     11,02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Active Calories (kcal)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  1.262,85</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      0,05</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    688,97</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    660,68</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance daily stats export by adding weekly and daily summary sheets in Excel format
</commit_message>
<xml_diff>
--- a/activity_summary.xlsx
+++ b/activity_summary.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -709,6 +709,46 @@
       <c r="D14" t="inlineStr">
         <is>
           <t xml:space="preserve">    677,50</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>13342</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      9,06</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    541,38</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>16025</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     10,33</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    557,36</t>
         </is>
       </c>
     </row>
@@ -806,16 +846,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45866</v>
+        <v>75233</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">     30,40</t>
+          <t xml:space="preserve">     49,79</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  1.738,45</t>
+          <t xml:space="preserve">  2.837,18</t>
         </is>
       </c>
     </row>
@@ -886,7 +926,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>218.569,00</t>
+          <t>247.936,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -901,12 +941,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17.625,00</t>
+          <t xml:space="preserve"> 17.609,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 16.813,00</t>
+          <t xml:space="preserve"> 16.529,07</t>
         </is>
       </c>
     </row>
@@ -918,7 +958,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    145,14</t>
+          <t xml:space="preserve">    164,53</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -933,12 +973,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     11,75</t>
+          <t xml:space="preserve">     11,73</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     11,16</t>
+          <t xml:space="preserve">     10,97</t>
         </is>
       </c>
     </row>
@@ -950,7 +990,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.718,37</t>
+          <t xml:space="preserve">  9.817,10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -965,12 +1005,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    698,96</t>
+          <t xml:space="preserve">    695,10</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    670,64</t>
+          <t xml:space="preserve">    654,47</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1083,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>218.569,00</t>
+          <t>247.936,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1068,12 +1108,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 17.625,00</t>
+          <t xml:space="preserve"> 17.609,00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 16.813,00</t>
+          <t xml:space="preserve"> 16.529,07</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1125,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    145,14</t>
+          <t xml:space="preserve">    164,53</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1110,12 +1150,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     11,75</t>
+          <t xml:space="preserve">     11,73</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">     11,16</t>
+          <t xml:space="preserve">     10,97</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1167,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  8.718,37</t>
+          <t xml:space="preserve">  9.817,10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1152,12 +1192,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    698,96</t>
+          <t xml:space="preserve">    695,10</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    670,64</t>
+          <t xml:space="preserve">    654,47</t>
         </is>
       </c>
     </row>
@@ -1184,7 +1224,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-15</t>
         </is>
       </c>
     </row>

</xml_diff>